<commit_message>
Update BG files, reinstate articulation test button.
</commit_message>
<xml_diff>
--- a/Doc/AppResources.xlsx
+++ b/Doc/AppResources.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\projects\speechpathology\softqnr\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\projects\SpeechPath\speechpathology\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9491712B-C376-4F07-96C0-0233CF2638E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30940" windowHeight="17500"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="sl" sheetId="2" r:id="rId3"/>
     <sheet name="nl" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="486">
   <si>
     <t>Worksheet saved.</t>
   </si>
@@ -1274,9 +1273,6 @@
   </si>
   <si>
     <t>Езикови умения</t>
-  </si>
-  <si>
-    <t>месеца</t>
   </si>
   <si>
     <t>месец</t>
@@ -1524,73 +1520,73 @@
     </r>
   </si>
   <si>
-    <t>Възраст на датата на теста</t>
-  </si>
-  <si>
-    <t>Тест спрямо възрастта</t>
-  </si>
-  <si>
-    <t>Възраст на детето</t>
-  </si>
-  <si>
-    <t>Не сте задали възраст за теста или възрастта, която сте посочили, е твърде малка. Моля, въведете валидна дата на раждане.</t>
-  </si>
-  <si>
-    <t>Възраст, която не се тества</t>
-  </si>
-  <si>
-    <t>Всички</t>
-  </si>
-  <si>
-    <t>Смесвам</t>
-  </si>
-  <si>
     <t>Смесен</t>
   </si>
   <si>
-    <t>Продължи</t>
-  </si>
-  <si>
-    <t>Говорни езикови умения</t>
-  </si>
-  <si>
-    <t>Букви</t>
-  </si>
-  <si>
-    <t>Ок</t>
-  </si>
-  <si>
-    <t>Инструменти за речева патология</t>
-  </si>
-  <si>
     <t>Резултати</t>
   </si>
   <si>
-    <t>Наличен е предходен тест</t>
-  </si>
-  <si>
-    <t>Запази</t>
-  </si>
-  <si>
     <t>Споделете речевите способности</t>
   </si>
   <si>
-    <t>Развитие на звуковото произношение</t>
-  </si>
-  <si>
-    <t>Речеви звуци</t>
-  </si>
-  <si>
-    <t>Продължете теста</t>
-  </si>
-  <si>
-    <t>Развитие на произношението според възрастта</t>
+    <t>Възраст в деня на теста</t>
+  </si>
+  <si>
+    <t>Тест базиран на възрастта</t>
+  </si>
+  <si>
+    <t>Възраст на ученика</t>
+  </si>
+  <si>
+    <t>Не сте конфигурирали приложението с възрастта за теста или възрастта, която сте задали, е твърде млада. Моля, въведете валидна дата на раждане.</t>
+  </si>
+  <si>
+    <t>Възраст, която не може да се тества</t>
+  </si>
+  <si>
+    <t>всички</t>
+  </si>
+  <si>
+    <t>бленда</t>
+  </si>
+  <si>
+    <t>Устни езикови умения</t>
+  </si>
+  <si>
+    <t>ок</t>
+  </si>
+  <si>
+    <t>Беше намерен предишен тест</t>
+  </si>
+  <si>
+    <t>запази</t>
+  </si>
+  <si>
+    <t>Развитие на речта</t>
+  </si>
+  <si>
+    <t>Звуци на речта</t>
+  </si>
+  <si>
+    <t>Продължете с теста</t>
+  </si>
+  <si>
+    <t>Прогрес на звука по време на възрастта</t>
+  </si>
+  <si>
+    <t>тест</t>
+  </si>
+  <si>
+    <t>Продължавам</t>
+  </si>
+  <si>
+    <t>Писма</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1631,7 +1627,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1641,6 +1637,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1659,7 +1661,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1697,10 +1699,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Navadno 2" xfId="2" xr:uid="{392453A2-7DC5-4ECF-861F-4592646E2465}"/>
-    <cellStyle name="Navadno 3" xfId="1" xr:uid="{6BE72BAF-2412-4362-855F-864B4BC8A7CC}"/>
+    <cellStyle name="Navadno 2" xfId="2"/>
+    <cellStyle name="Navadno 3" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2012,25 +2017,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="34.21875" style="14" customWidth="1"/>
-    <col min="4" max="4" width="34.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="34.21875" customWidth="1"/>
-    <col min="6" max="6" width="34.21875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="34.21875" customWidth="1"/>
+    <col min="1" max="1" width="20.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="34.1796875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="34.1796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="34.1796875" customWidth="1"/>
+    <col min="6" max="6" width="34.1796875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="34.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>46</v>
       </c>
@@ -2053,14 +2058,14 @@
         <v>339</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -2076,14 +2081,14 @@
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -2099,14 +2104,14 @@
         <v>282</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="10" t="s">
         <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -2122,14 +2127,14 @@
         <v>283</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="10" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -2145,15 +2150,15 @@
         <v>284</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>466</v>
+      <c r="C6" s="15" t="s">
+        <v>468</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>148</v>
@@ -2168,15 +2173,15 @@
         <v>285</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>467</v>
+      <c r="C7" s="5" t="s">
+        <v>469</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>149</v>
@@ -2191,15 +2196,15 @@
         <v>286</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>468</v>
+      <c r="C8" s="5" t="s">
+        <v>470</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>150</v>
@@ -2214,15 +2219,15 @@
         <v>287</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>469</v>
+      <c r="C9" s="5" t="s">
+        <v>471</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>151</v>
@@ -2237,15 +2242,15 @@
         <v>288</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>470</v>
+      <c r="C10" s="5" t="s">
+        <v>472</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>152</v>
@@ -2260,15 +2265,15 @@
         <v>289</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>153</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>471</v>
+      <c r="C11" s="5" t="s">
+        <v>473</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>153</v>
@@ -2283,14 +2288,14 @@
         <v>290</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="10" t="s">
         <v>141</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -2306,14 +2311,14 @@
         <v>291</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -2329,15 +2334,15 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>472</v>
+      <c r="C14" s="5" t="s">
+        <v>474</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>156</v>
@@ -2352,15 +2357,15 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>157</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>473</v>
+      <c r="C15" s="5" t="s">
+        <v>465</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>158</v>
@@ -2375,14 +2380,14 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="10" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -2398,15 +2403,15 @@
         <v>294</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>474</v>
+      <c r="C17" s="5" t="s">
+        <v>484</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>160</v>
@@ -2421,14 +2426,14 @@
         <v>295</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="10" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -2444,14 +2449,14 @@
         <v>340</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="5" t="s">
         <v>407</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -2467,14 +2472,14 @@
         <v>296</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="5" t="s">
         <v>408</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -2490,14 +2495,14 @@
         <v>297</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="15" t="s">
         <v>409</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -2513,14 +2518,14 @@
         <v>298</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="5" t="s">
         <v>410</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -2536,14 +2541,14 @@
         <v>298</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -2559,14 +2564,14 @@
         <v>299</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="10" t="s">
         <v>37</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -2582,14 +2587,14 @@
         <v>300</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -2605,14 +2610,14 @@
         <v>301</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -2628,14 +2633,14 @@
         <v>302</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="10" t="s">
         <v>18</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -2651,14 +2656,14 @@
         <v>341</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -2674,14 +2679,14 @@
         <v>303</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="5" t="s">
         <v>475</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -2697,14 +2702,14 @@
         <v>304</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="5" t="s">
         <v>411</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -2720,15 +2725,15 @@
         <v>304</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>172</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C31" s="14" t="s">
-        <v>476</v>
+      <c r="C31" s="5" t="s">
+        <v>485</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>172</v>
@@ -2743,14 +2748,14 @@
         <v>172</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="10" t="s">
         <v>24</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -2766,14 +2771,14 @@
         <v>305</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -2789,14 +2794,14 @@
         <v>306</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="10" t="s">
         <v>40</v>
       </c>
       <c r="D34" s="2" t="s">
@@ -2812,15 +2817,15 @@
         <v>307</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="14" t="s">
-        <v>412</v>
+      <c r="C35" s="15" t="s">
+        <v>246</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>175</v>
@@ -2835,15 +2840,15 @@
         <v>308</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C36" s="14" t="s">
-        <v>413</v>
+      <c r="C36" s="5" t="s">
+        <v>412</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>176</v>
@@ -2858,14 +2863,14 @@
         <v>308</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="10" t="s">
         <v>142</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -2881,15 +2886,15 @@
         <v>309</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>178</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C38" s="14" t="s">
-        <v>477</v>
+      <c r="C38" s="15" t="s">
+        <v>476</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>179</v>
@@ -2904,14 +2909,14 @@
         <v>179</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="10" t="s">
         <v>33</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -2927,14 +2932,14 @@
         <v>310</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="10" t="s">
         <v>35</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -2950,14 +2955,14 @@
         <v>311</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C41" s="10" t="s">
         <v>22</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -2973,14 +2978,14 @@
         <v>312</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="10" t="s">
         <v>44</v>
       </c>
       <c r="D42" s="2" t="s">
@@ -2996,15 +3001,15 @@
         <v>313</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C43" s="14" t="s">
-        <v>478</v>
+      <c r="C43" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>184</v>
@@ -3019,14 +3024,14 @@
         <v>314</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -3042,14 +3047,14 @@
         <v>315</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="10" t="s">
         <v>23</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -3065,15 +3070,15 @@
         <v>316</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>187</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C46" s="14" t="s">
-        <v>479</v>
+      <c r="C46" s="10" t="s">
+        <v>466</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>188</v>
@@ -3088,15 +3093,15 @@
         <v>317</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>189</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="C47" s="14" t="s">
-        <v>414</v>
+      <c r="C47" s="5" t="s">
+        <v>413</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>190</v>
@@ -3111,15 +3116,15 @@
         <v>318</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>191</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="C48" s="14" t="s">
-        <v>480</v>
+      <c r="C48" s="15" t="s">
+        <v>477</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>192</v>
@@ -3134,15 +3139,15 @@
         <v>319</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>193</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C49" s="14" t="s">
-        <v>481</v>
+      <c r="C49" s="15" t="s">
+        <v>478</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>194</v>
@@ -3157,14 +3162,14 @@
         <v>320</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>195</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C50" s="5" t="s">
         <v>255</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -3180,14 +3185,14 @@
         <v>321</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="C51" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D51" s="2" t="s">
@@ -3203,14 +3208,14 @@
         <v>322</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="C52" s="10" t="s">
         <v>20</v>
       </c>
       <c r="D52" s="2" t="s">
@@ -3226,14 +3231,14 @@
         <v>323</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="C53" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D53" s="2" t="s">
@@ -3249,14 +3254,14 @@
         <v>324</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="C54" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D54" s="2" t="s">
@@ -3272,7 +3277,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>120</v>
       </c>
@@ -3280,7 +3285,7 @@
         <v>121</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>482</v>
+        <v>467</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>200</v>
@@ -3295,14 +3300,14 @@
         <v>326</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C56" s="14" t="s">
+      <c r="C56" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D56" s="2" t="s">
@@ -3318,14 +3323,14 @@
         <v>327</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>123</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="14" t="s">
+      <c r="C57" s="10" t="s">
         <v>32</v>
       </c>
       <c r="D57" s="2" t="s">
@@ -3341,14 +3346,14 @@
         <v>328</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C58" s="14" t="s">
+      <c r="C58" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D58" s="2" t="s">
@@ -3364,14 +3369,14 @@
         <v>329</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="14" t="s">
+      <c r="C59" s="10" t="s">
         <v>34</v>
       </c>
       <c r="D59" s="2" t="s">
@@ -3387,15 +3392,15 @@
         <v>330</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C60" s="14" t="s">
-        <v>483</v>
+      <c r="C60" s="5" t="s">
+        <v>479</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>205</v>
@@ -3410,15 +3415,15 @@
         <v>331</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C61" s="14" t="s">
-        <v>484</v>
+      <c r="C61" s="5" t="s">
+        <v>480</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>206</v>
@@ -3433,15 +3438,15 @@
         <v>331</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>130</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C62" s="14" t="s">
-        <v>485</v>
+      <c r="C62" s="5" t="s">
+        <v>481</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>207</v>
@@ -3456,15 +3461,15 @@
         <v>318</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C63" s="14" t="s">
-        <v>486</v>
+      <c r="C63" s="5" t="s">
+        <v>482</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>208</v>
@@ -3479,15 +3484,15 @@
         <v>332</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>209</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C64" s="14" t="s">
-        <v>273</v>
+      <c r="C64" s="5" t="s">
+        <v>483</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>209</v>
@@ -3502,14 +3507,14 @@
         <v>209</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>134</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C65" s="14" t="s">
+      <c r="C65" s="10" t="s">
         <v>16</v>
       </c>
       <c r="D65" s="2" t="s">
@@ -3525,14 +3530,14 @@
         <v>333</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C66" s="14" t="s">
+      <c r="C66" s="10" t="s">
         <v>25</v>
       </c>
       <c r="D66" s="2" t="s">
@@ -3548,14 +3553,14 @@
         <v>334</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>136</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C67" s="14" t="s">
+      <c r="C67" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D67" s="2" t="s">
@@ -3571,15 +3576,15 @@
         <v>335</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C68" s="14" t="s">
-        <v>415</v>
+      <c r="C68" s="5" t="s">
+        <v>414</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>213</v>
@@ -3594,14 +3599,14 @@
         <v>336</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>139</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C69" s="14" t="s">
+      <c r="C69" s="5" t="s">
         <v>278</v>
       </c>
       <c r="D69" s="2" t="s">
@@ -3624,20 +3629,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B65133-C3B7-48ED-B9DD-DCBF27A313D6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B69" sqref="A2:B69"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.21875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="20.90625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.453125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="34.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>46</v>
       </c>
@@ -3645,503 +3651,503 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="10" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="10" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" s="10" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" s="10" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="10" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="10" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B14" s="10" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="B15" s="14" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" s="10" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="14" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="10" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="10" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="10" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="10" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="10" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="10" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="10" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="B31" s="14" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B31" s="10" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B35" s="14" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="14" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="10" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="10" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="B38" s="14" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B38" s="10" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B43" s="14" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B43" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="B46" s="14" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B46" s="10" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="B47" s="14" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B47" s="10" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="B48" s="14" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B48" s="10" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="B49" s="14" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="10" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="10" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B55" s="14" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B55" s="10" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B60" s="14" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B60" s="10" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B61" s="14" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B61" s="10" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B62" s="14" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B62" s="10" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B63" s="14" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B63" s="10" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
         <v>209</v>
       </c>
@@ -4149,43 +4155,43 @@
         <v>273</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B67" s="14" t="s">
+      <c r="B67" s="10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="B68" s="14" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B68" s="10" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B69" s="14" t="s">
+      <c r="B69" s="10" t="s">
         <v>278</v>
       </c>
     </row>
@@ -4195,20 +4201,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3324D98B-3BB6-4216-90AE-36C96065F197}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.21875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="20.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1796875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>46</v>
       </c>
@@ -4216,31 +4222,31 @@
         <v>279</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
@@ -4248,47 +4254,47 @@
         <v>345</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>153</v>
       </c>
@@ -4296,23 +4302,23 @@
         <v>351</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>67</v>
       </c>
@@ -4320,7 +4326,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>157</v>
       </c>
@@ -4328,7 +4334,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
@@ -4336,7 +4342,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>70</v>
       </c>
@@ -4344,7 +4350,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>71</v>
       </c>
@@ -4352,7 +4358,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -4360,7 +4366,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>74</v>
       </c>
@@ -4368,15 +4374,15 @@
         <v>359</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>78</v>
       </c>
@@ -4384,39 +4390,39 @@
         <v>361</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>85</v>
       </c>
@@ -4424,55 +4430,55 @@
         <v>365</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>172</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>96</v>
       </c>
@@ -4480,7 +4486,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>97</v>
       </c>
@@ -4488,7 +4494,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>99</v>
       </c>
@@ -4496,15 +4502,15 @@
         <v>373</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>178</v>
       </c>
@@ -4512,7 +4518,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>103</v>
       </c>
@@ -4520,39 +4526,39 @@
         <v>376</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>110</v>
       </c>
@@ -4560,15 +4566,15 @@
         <v>381</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>187</v>
       </c>
@@ -4576,23 +4582,23 @@
         <v>383</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>189</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>191</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>193</v>
       </c>
@@ -4600,71 +4606,71 @@
         <v>386</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>195</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>123</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>124</v>
       </c>
@@ -4672,55 +4678,55 @@
         <v>395</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>130</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>209</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>134</v>
       </c>
@@ -4728,23 +4734,23 @@
         <v>401</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>136</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>137</v>
       </c>
@@ -4752,7 +4758,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>139</v>
       </c>
@@ -4766,20 +4772,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7AEF2E1-26D9-4E26-B917-9A3C6ACE91C6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="20.90625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.453125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>46</v>
       </c>
@@ -4787,7 +4793,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>48</v>
       </c>
@@ -4795,15 +4801,15 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>50</v>
       </c>
@@ -4811,7 +4817,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>51</v>
       </c>
@@ -4819,7 +4825,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>53</v>
       </c>
@@ -4827,7 +4833,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>55</v>
       </c>
@@ -4835,7 +4841,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>57</v>
       </c>
@@ -4843,7 +4849,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>59</v>
       </c>
@@ -4851,7 +4857,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>61</v>
       </c>
@@ -4859,23 +4865,23 @@
         <v>152</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>153</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>63</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>65</v>
       </c>
@@ -4883,7 +4889,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>67</v>
       </c>
@@ -4891,7 +4897,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>157</v>
       </c>
@@ -4899,7 +4905,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>69</v>
       </c>
@@ -4907,7 +4913,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>70</v>
       </c>
@@ -4915,7 +4921,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>71</v>
       </c>
@@ -4923,7 +4929,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>72</v>
       </c>
@@ -4931,7 +4937,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>74</v>
       </c>
@@ -4939,7 +4945,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>76</v>
       </c>
@@ -4947,7 +4953,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>78</v>
       </c>
@@ -4955,7 +4961,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>5</v>
       </c>
@@ -4963,7 +4969,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>80</v>
       </c>
@@ -4971,7 +4977,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>82</v>
       </c>
@@ -4979,7 +4985,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>83</v>
       </c>
@@ -4987,7 +4993,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>85</v>
       </c>
@@ -4995,7 +5001,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>86</v>
       </c>
@@ -5003,7 +5009,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>88</v>
       </c>
@@ -5011,7 +5017,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>90</v>
       </c>
@@ -5019,7 +5025,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>172</v>
       </c>
@@ -5027,7 +5033,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>92</v>
       </c>
@@ -5035,7 +5041,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>94</v>
       </c>
@@ -5043,7 +5049,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>96</v>
       </c>
@@ -5051,7 +5057,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>97</v>
       </c>
@@ -5059,7 +5065,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>99</v>
       </c>
@@ -5067,7 +5073,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>101</v>
       </c>
@@ -5075,7 +5081,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>178</v>
       </c>
@@ -5083,7 +5089,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>103</v>
       </c>
@@ -5091,7 +5097,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>104</v>
       </c>
@@ -5099,7 +5105,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>105</v>
       </c>
@@ -5107,7 +5113,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>106</v>
       </c>
@@ -5115,7 +5121,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
         <v>108</v>
       </c>
@@ -5123,7 +5129,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
         <v>110</v>
       </c>
@@ -5131,7 +5137,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
         <v>112</v>
       </c>
@@ -5139,7 +5145,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
         <v>187</v>
       </c>
@@ -5147,7 +5153,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
         <v>189</v>
       </c>
@@ -5155,7 +5161,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
         <v>191</v>
       </c>
@@ -5163,7 +5169,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
         <v>193</v>
       </c>
@@ -5171,7 +5177,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="7" t="s">
         <v>195</v>
       </c>
@@ -5179,7 +5185,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
         <v>114</v>
       </c>
@@ -5187,7 +5193,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
         <v>116</v>
       </c>
@@ -5195,7 +5201,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="7" t="s">
         <v>118</v>
       </c>
@@ -5203,15 +5209,15 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
         <v>119</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
         <v>120</v>
       </c>
@@ -5219,7 +5225,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>122</v>
       </c>
@@ -5227,7 +5233,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
         <v>123</v>
       </c>
@@ -5235,7 +5241,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
         <v>124</v>
       </c>
@@ -5243,7 +5249,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
         <v>125</v>
       </c>
@@ -5251,7 +5257,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
         <v>126</v>
       </c>
@@ -5259,7 +5265,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
         <v>128</v>
       </c>
@@ -5267,7 +5273,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
         <v>130</v>
       </c>
@@ -5275,15 +5281,15 @@
         <v>207</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
         <v>132</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
         <v>209</v>
       </c>
@@ -5291,7 +5297,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
         <v>134</v>
       </c>
@@ -5299,7 +5305,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="7" t="s">
         <v>135</v>
       </c>
@@ -5307,7 +5313,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="7" t="s">
         <v>136</v>
       </c>
@@ -5315,7 +5321,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="7" t="s">
         <v>137</v>
       </c>
@@ -5323,7 +5329,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="7" t="s">
         <v>139</v>
       </c>

</xml_diff>

<commit_message>
Updating db for months
Add LetterFocus field for articulation test
</commit_message>
<xml_diff>
--- a/Doc/AppResources.xlsx
+++ b/Doc/AppResources.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30940" windowHeight="17500" activeTab="5"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30940" windowHeight="17500"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1336" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="454">
   <si>
     <t>Worksheet saved.</t>
   </si>
@@ -1462,6 +1462,30 @@
   </si>
   <si>
     <t xml:space="preserve"> od </t>
+  </si>
+  <si>
+    <t>LetterFocus</t>
+  </si>
+  <si>
+    <t>Does your child pronounce {0} correctly?</t>
+  </si>
+  <si>
+    <t>Произнася ли детето {0} правилно?</t>
+  </si>
+  <si>
+    <t>Spreekt uw kind de {0} correct uit?</t>
+  </si>
+  <si>
+    <t>Да ли ваше дијете исправно изговара {0}?</t>
+  </si>
+  <si>
+    <t>Ali vaš otrok pravilno izgovori {0}?</t>
+  </si>
+  <si>
+    <t>Çocuğunuz {0} doğru telaffuz ediyor mu?</t>
+  </si>
+  <si>
+    <t>Harfler</t>
   </si>
 </sst>
 </file>
@@ -1548,7 +1572,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1611,6 +1635,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1929,10 +1960,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2636,139 +2668,139 @@
         <v>296</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>429</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="F31" s="25" t="s">
-        <v>379</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>166</v>
+    <row r="31" spans="1:7" s="26" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="26" t="s">
+        <v>446</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>447</v>
+      </c>
+      <c r="C31" s="27" t="s">
+        <v>448</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>449</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>450</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>451</v>
+      </c>
+      <c r="G31" s="27" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>89</v>
+        <v>166</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>24</v>
+        <v>166</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>429</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="F32" s="24" t="s">
-        <v>380</v>
+        <v>166</v>
+      </c>
+      <c r="F32" s="25" t="s">
+        <v>379</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>297</v>
+        <v>453</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>441</v>
+        <v>167</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>154</v>
+        <v>441</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>336</v>
+        <v>381</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>239</v>
+        <v>92</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>359</v>
+        <v>94</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>239</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>239</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>300</v>
@@ -2776,788 +2808,811 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>439</v>
+        <v>96</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>359</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="F37" s="15" t="s">
-        <v>445</v>
+        <v>239</v>
+      </c>
+      <c r="F37" s="24" t="s">
+        <v>345</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>171</v>
+        <v>97</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>420</v>
+        <v>98</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>439</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F38" s="25" t="s">
-        <v>171</v>
+        <v>240</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>445</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>172</v>
+        <v>301</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>99</v>
+        <v>171</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>33</v>
+        <v>172</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>420</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="F39" s="24" t="s">
-        <v>346</v>
+        <v>172</v>
+      </c>
+      <c r="F39" s="25" t="s">
+        <v>171</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>302</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>382</v>
+        <v>346</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F41" s="24" t="s">
+        <v>382</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C42" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="F41" s="24" t="s">
+      <c r="F42" s="24" t="s">
         <v>383</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>304</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="F42" s="24" t="s">
-        <v>384</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="F43" s="24" t="s">
+        <v>384</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C44" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="F43" s="24" t="s">
+      <c r="F44" s="24" t="s">
         <v>444</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G44" s="2" t="s">
         <v>306</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="F44" s="24" t="s">
-        <v>347</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>23</v>
+        <v>107</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>385</v>
+        <v>347</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="F46" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C47" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="F46" s="24" t="s">
+      <c r="F47" s="24" t="s">
         <v>348</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G47" s="2" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
+    <row r="48" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C48" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="F47" s="25" t="s">
+      <c r="F48" s="25" t="s">
         <v>386</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G48" s="2" t="s">
         <v>310</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>421</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="F48" s="25" t="s">
-        <v>387</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>186</v>
+        <v>330</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="F49" s="24" t="s">
-        <v>349</v>
+        <v>250</v>
+      </c>
+      <c r="F49" s="25" t="s">
+        <v>387</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>422</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F50" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C51" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="E51" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="F50" s="25" t="s">
+      <c r="F51" s="25" t="s">
         <v>388</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="G51" s="2" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C52" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="F51" s="24" t="s">
+      <c r="F52" s="24" t="s">
         <v>389</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="G52" s="2" t="s">
         <v>314</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="F52" s="24" t="s">
-        <v>390</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>4</v>
+        <v>113</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F54" s="24" t="s">
+        <v>391</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C55" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="F54" s="24" t="s">
+      <c r="F55" s="24" t="s">
         <v>392</v>
       </c>
-      <c r="G54" s="2" t="s">
+      <c r="G55" s="2" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C56" s="12" t="s">
         <v>411</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E56" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="F55" s="24" t="s">
+      <c r="F56" s="24" t="s">
         <v>393</v>
       </c>
-      <c r="G55" s="2" t="s">
+      <c r="G56" s="2" t="s">
         <v>318</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="F56" s="24" t="s">
-        <v>394</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F57" s="24" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F58" s="24" t="s">
+        <v>395</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C59" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="F58" s="24" t="s">
+      <c r="F59" s="24" t="s">
         <v>350</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="G59" s="2" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="59" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="6" t="s">
+    <row r="60" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B59" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="F59" s="24" t="s">
-        <v>396</v>
-      </c>
-      <c r="G59" s="9" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A60" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C60" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D60" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="E60" s="9" t="s">
         <v>261</v>
       </c>
       <c r="F60" s="24" t="s">
         <v>396</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>436</v>
+        <v>322</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>122</v>
+        <v>434</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>423</v>
+        <v>10</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>323</v>
+        <v>436</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>437</v>
+        <v>323</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="F63" s="24" t="s">
+        <v>398</v>
+      </c>
+      <c r="G63" s="9" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C64" s="5" t="s">
         <v>425</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="E64" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="F63" s="24" t="s">
+      <c r="F64" s="24" t="s">
         <v>399</v>
       </c>
-      <c r="G63" s="2" t="s">
+      <c r="G64" s="2" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C65" s="5" t="s">
         <v>426</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="E65" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="F64" s="24" t="s">
+      <c r="F65" s="24" t="s">
         <v>400</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="G65" s="2" t="s">
         <v>324</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>427</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="F65" s="24" t="s">
-        <v>401</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>130</v>
+        <v>202</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>16</v>
+        <v>202</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>427</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F66" s="24" t="s">
-        <v>351</v>
+        <v>401</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>325</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F67" s="24" t="s">
-        <v>402</v>
+        <v>351</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F68" s="24" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>361</v>
+        <v>12</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F69" s="24" t="s">
-        <v>352</v>
+        <v>403</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>271</v>
+        <v>361</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F70" s="24" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F71" s="16"/>
+      <c r="A71" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F71" s="24" t="s">
+        <v>353</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F72" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3567,11 +3622,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3820,113 +3873,113 @@
         <v>358</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>429</v>
+    <row r="31" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="20" t="s">
+        <v>446</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
-        <v>89</v>
+        <v>166</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>24</v>
+        <v>429</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>239</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>359</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>138</v>
+        <v>359</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
-        <v>171</v>
+        <v>97</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>420</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
-        <v>99</v>
+        <v>171</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>33</v>
+        <v>420</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>36</v>
@@ -3934,127 +3987,127 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
-        <v>180</v>
+        <v>108</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>410</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>360</v>
+        <v>410</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>421</v>
+        <v>360</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>248</v>
+        <v>422</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
-        <v>110</v>
+        <v>188</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>19</v>
+        <v>248</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>411</v>
+        <v>30</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>31</v>
+        <v>411</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B59" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="6" t="s">
+    <row r="60" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="B59" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" s="6" t="s">
-        <v>434</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>34</v>
@@ -4062,81 +4115,89 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="6" t="s">
-        <v>122</v>
+        <v>434</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>423</v>
+        <v>34</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B63" s="9" t="s">
+      <c r="B64" s="9" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="6" t="s">
+    <row r="65" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A65" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B65" s="9" t="s">
         <v>426</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>16</v>
+        <v>202</v>
+      </c>
+      <c r="B66" s="12" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>361</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="B71" s="9" t="s">
         <v>271</v>
       </c>
     </row>
@@ -4147,11 +4208,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B72"/>
+  <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4407,249 +4466,249 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>166</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>166</v>
+    <row r="32" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="20" t="s">
+        <v>446</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>89</v>
+        <v>166</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>90</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>432</v>
+        <v>95</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>433</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>432</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>98</v>
+        <v>433</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>171</v>
+        <v>97</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>172</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>99</v>
+        <v>171</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>9</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>101</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>180</v>
+        <v>108</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>180</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>329</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>186</v>
+        <v>330</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>110</v>
+        <v>188</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>111</v>
+        <v>188</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>4</v>
+        <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>117</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>7</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>10</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>434</v>
+        <v>121</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>10</v>
@@ -4657,81 +4716,89 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>122</v>
+        <v>434</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>123</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>202</v>
+        <v>128</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>202</v>
+        <v>129</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>130</v>
+        <v>202</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>130</v>
+        <v>202</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>0</v>
+        <v>130</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>134</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
+        <v>133</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
         <v>135</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="B73" s="9" t="s">
         <v>136</v>
       </c>
     </row>
@@ -4743,11 +4810,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B69"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4995,315 +5060,323 @@
         <v>165</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>166</v>
+    <row r="31" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="20" t="s">
+        <v>446</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
-        <v>89</v>
+        <v>166</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>441</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>154</v>
+        <v>441</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
-        <v>171</v>
+        <v>97</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
-        <v>99</v>
+        <v>171</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
-        <v>180</v>
+        <v>108</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
-        <v>110</v>
+        <v>188</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>407</v>
+        <v>191</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>193</v>
+        <v>407</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>408</v>
+        <v>200</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="6" t="s">
-        <v>202</v>
+        <v>128</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>202</v>
+        <v>408</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="6" t="s">
-        <v>130</v>
+        <v>202</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B69" s="9" t="s">
+      <c r="B70" s="9" t="s">
         <v>207</v>
       </c>
     </row>
@@ -5315,11 +5388,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -5567,49 +5638,49 @@
         <v>236</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" s="20" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="20" t="s">
-        <v>166</v>
+        <v>446</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>166</v>
+        <v>450</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="20" t="s">
-        <v>89</v>
+        <v>166</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>237</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B36" s="21" t="s">
         <v>239</v>
@@ -5617,191 +5688,191 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="20" t="s">
-        <v>171</v>
+        <v>97</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>172</v>
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="20" t="s">
-        <v>99</v>
+        <v>171</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>241</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="B46" s="21" t="s">
+      <c r="B47" s="21" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="20" t="s">
+    <row r="48" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A48" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="B47" s="21" t="s">
+      <c r="B48" s="21" t="s">
         <v>249</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="B48" s="21" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="20" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="B50" s="21" t="s">
+      <c r="B51" s="21" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A51" s="20" t="s">
+    <row r="52" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A52" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="B51" s="21" t="s">
+      <c r="B52" s="21" t="s">
         <v>253</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="B52" s="21" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="B54" s="21" t="s">
+      <c r="B55" s="21" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A55" s="20" t="s">
+    <row r="56" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A56" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="B55" s="21" t="s">
+      <c r="B56" s="21" t="s">
         <v>257</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="B56" s="21" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B57" s="21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="20" t="s">
-        <v>434</v>
+        <v>121</v>
       </c>
       <c r="B60" s="21" t="s">
         <v>261</v>
@@ -5809,81 +5880,89 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="20" t="s">
-        <v>122</v>
+        <v>434</v>
       </c>
       <c r="B61" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B63" s="21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="20" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="20" t="s">
-        <v>202</v>
+        <v>128</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="20" t="s">
-        <v>130</v>
+        <v>202</v>
       </c>
       <c r="B66" s="21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B67" s="21" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B68" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B69" s="21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B70" s="21" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="B70" s="21" t="s">
+      <c r="B71" s="21" t="s">
         <v>271</v>
       </c>
     </row>
@@ -5894,11 +5973,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -6147,241 +6224,241 @@
         <v>378</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>166</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>379</v>
+    <row r="31" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="20" t="s">
+        <v>446</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>89</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>380</v>
+        <v>166</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>336</v>
+        <v>381</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>97</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>445</v>
+        <v>95</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>171</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>171</v>
+        <v>97</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>99</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>346</v>
+        <v>171</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>382</v>
+        <v>346</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>102</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B43" s="17" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="44" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>104</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B44" s="17" t="s">
         <v>444</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>106</v>
-      </c>
-      <c r="B44" s="17" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>385</v>
+        <v>347</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>180</v>
+        <v>108</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>348</v>
+        <v>385</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>182</v>
-      </c>
-      <c r="B47" s="19" t="s">
-        <v>386</v>
+        <v>180</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>186</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>349</v>
+        <v>184</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>188</v>
-      </c>
-      <c r="B50" s="19" t="s">
-        <v>388</v>
+        <v>186</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>110</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>389</v>
+        <v>188</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>119</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>120</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B59" s="17" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="59" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="6" t="s">
+    <row r="60" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="B59" s="17" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>434</v>
       </c>
       <c r="B60" s="17" t="s">
         <v>396</v>
@@ -6389,86 +6466,94 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>122</v>
+        <v>434</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>202</v>
+        <v>128</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>130</v>
+        <v>202</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>351</v>
+        <v>401</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>402</v>
+        <v>351</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>352</v>
+        <v>403</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>133</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
         <v>135</v>
       </c>
-      <c r="B70" s="17" t="s">
+      <c r="B71" s="17" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B71"/>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B72"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6477,11 +6562,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B72"/>
+  <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62:B64"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -6737,49 +6820,49 @@
         <v>435</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>166</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>166</v>
+    <row r="32" spans="1:2" s="20" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="20" t="s">
+        <v>446</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>89</v>
+        <v>166</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>297</v>
+        <v>453</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>300</v>
@@ -6787,281 +6870,289 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>432</v>
+        <v>95</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>433</v>
+        <v>300</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>432</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>301</v>
+        <v>433</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>171</v>
+        <v>97</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>172</v>
+        <v>301</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>99</v>
+        <v>171</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>302</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>180</v>
+        <v>108</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>110</v>
+        <v>188</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>434</v>
+        <v>121</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>436</v>
+        <v>322</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>122</v>
+        <v>434</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>323</v>
+        <v>436</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>437</v>
+        <v>323</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>310</v>
+        <v>437</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>202</v>
+        <v>128</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>202</v>
+        <v>324</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>130</v>
+        <v>202</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>325</v>
+        <v>202</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
+        <v>133</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
         <v>135</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="B73" s="9" t="s">
         <v>328</v>
       </c>
     </row>

</xml_diff>